<commit_message>
participant 105 data processing
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lab/Documents/GitHub/rejection_risk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA134B7-66ED-524F-9948-A5394C14A9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B20A26-30DA-AB46-80F9-92C1B2ED722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="3700" windowWidth="27240" windowHeight="16440" xr2:uid="{AE79E526-0397-D443-9F8C-69B922399B52}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>R_69lCvNl5MnCGgzD</t>
+  </si>
+  <si>
+    <t>R_34L7XTVaE312VgJ</t>
+  </si>
+  <si>
+    <t>R_6pffiNtHXao5FYL</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD9EDE5-C33C-8749-88FC-31AB8BB955C0}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,6 +510,23 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B5">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
106 and 108 data processing
</commit_message>
<xml_diff>
--- a/participantlist.xlsx
+++ b/participantlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lab/Documents/GitHub/rejection_risk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B20A26-30DA-AB46-80F9-92C1B2ED722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91878D87-9F42-1A46-AED3-E804E169C32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14520" yWindow="3700" windowWidth="27240" windowHeight="16440" xr2:uid="{AE79E526-0397-D443-9F8C-69B922399B52}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>R_6pffiNtHXao5FYL</t>
+  </si>
+  <si>
+    <t>R_1kNcuYDMTmIPVBg</t>
+  </si>
+  <si>
+    <t>R_325Icq7AOez25LX</t>
+  </si>
+  <si>
+    <t>R_3VL7UmQBWN0n2Xn</t>
+  </si>
+  <si>
+    <t>R_5NlSb3U49Wgqq9j</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD9EDE5-C33C-8749-88FC-31AB8BB955C0}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +539,59 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45972</v>
+      </c>
+      <c r="B6">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45972</v>
+      </c>
+      <c r="B8">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>